<commit_message>
Updates to Met Office Second Order stations
1895-1899 QCd
</commit_message>
<xml_diff>
--- a/second-order/1897/December1897.xlsx
+++ b/second-order/1897/December1897.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24202"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\catherine.ross\Desktop\2nd Order Stations\1896 - Copy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13594" documentId="13_ncr:1_{D72BFCFB-015C-4CD8-A97B-8AF3B863DC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7344CA19-EAED-494D-934A-7740864BC065}"/>
+  <xr:revisionPtr revIDLastSave="14352" documentId="13_ncr:1_{D72BFCFB-015C-4CD8-A97B-8AF3B863DC61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D91FFD6A-7923-493F-961B-DD4591A23C12}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="989" firstSheet="19" activeTab="20" xr2:uid="{F301734F-2AF4-4BAC-817B-B629B6303572}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="989" firstSheet="7" activeTab="20" xr2:uid="{F301734F-2AF4-4BAC-817B-B629B6303572}"/>
   </bookViews>
   <sheets>
     <sheet name="Deerness" sheetId="15" r:id="rId1"/>
@@ -47,6 +47,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -352,7 +354,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -529,11 +531,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -604,9 +615,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -638,6 +646,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -954,10 +968,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4108655-B436-409A-BEA1-C15E2C901F28}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="I37" sqref="I37"/>
+    <sheetView topLeftCell="N25" workbookViewId="0">
+      <selection activeCell="X31" sqref="X31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -970,66 +984,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -1037,67 +1041,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -1405,7 +1409,7 @@
         <v>29.72</v>
       </c>
       <c r="F9" s="5">
-        <v>20.61</v>
+        <v>29.61</v>
       </c>
       <c r="G9" s="1">
         <v>40.200000000000003</v>
@@ -3368,6 +3372,16 @@
       </c>
       <c r="W36" s="16">
         <v>3.7549999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37">
+        <f>SUM(E5:E35)/31</f>
+        <v>29.426451612903222</v>
+      </c>
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.41516129032258</v>
       </c>
     </row>
   </sheetData>
@@ -3391,8 +3405,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67F58535-F46B-4397-857F-B5B0AFE46BF9}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView topLeftCell="N31" workbookViewId="0">
+      <selection activeCell="V44" sqref="V44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3405,66 +3419,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -3472,67 +3476,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -5825,8 +5829,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6247AB03-F025-446C-8D2D-1CBADED51F88}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="V37" sqref="V37"/>
+    <sheetView topLeftCell="C25" workbookViewId="0">
+      <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5839,66 +5843,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -5906,67 +5900,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -7313,10 +7307,10 @@
         <v>2</v>
       </c>
       <c r="U23" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="V23" s="1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W23" s="11" t="s">
         <v>25</v>
@@ -8257,9 +8251,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CD0F272-B8A4-46FC-A472-771D73413392}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="P29" workbookViewId="0">
       <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
@@ -8273,66 +8267,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -8340,67 +8324,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -10671,6 +10655,12 @@
       </c>
       <c r="W36" s="16">
         <v>4.9669999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.255483870967741</v>
       </c>
     </row>
   </sheetData>
@@ -10693,8 +10683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD84A6CC-49D4-47FD-9DBF-F07FCE349F1A}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="Q32" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -10707,66 +10697,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -10774,67 +10754,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -13125,10 +13105,10 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F522100-1AF0-43D4-A080-F24B7139868C}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView topLeftCell="B24" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -13141,66 +13121,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -13208,67 +13178,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -14378,7 +14348,7 @@
         <v>3.2</v>
       </c>
       <c r="M20" s="4">
-        <v>0.54</v>
+        <v>0.34</v>
       </c>
       <c r="N20" s="5">
         <v>0.38600000000000001</v>
@@ -15539,6 +15509,12 @@
       </c>
       <c r="W36" s="16">
         <v>5.4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.797419354838706</v>
       </c>
     </row>
   </sheetData>
@@ -15559,10 +15535,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42ABBC7C-B157-4A4E-8414-C98E473BD393}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="R25" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -15575,66 +15551,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -15642,67 +15608,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -17973,6 +17939,16 @@
       </c>
       <c r="W36" s="16">
         <v>4.9349999999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37">
+        <f>SUM(E5:E35)/31</f>
+        <v>29.877419354838715</v>
+      </c>
+      <c r="J37">
+        <f>SUM(J5:J35)/31</f>
+        <v>48.290322580645167</v>
       </c>
     </row>
   </sheetData>
@@ -17995,7 +17971,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55D9C1B2-8C1C-4225-9D26-AF6DAC2640AF}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
+    <sheetView topLeftCell="U27" workbookViewId="0">
       <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
@@ -18009,66 +17985,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -18076,67 +18042,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -18850,7 +18816,7 @@
         <v>9</v>
       </c>
       <c r="W14" s="11">
-        <v>0.45</v>
+        <v>0.39</v>
       </c>
     </row>
     <row r="15" spans="1:23" s="1" customFormat="1">
@@ -20427,10 +20393,10 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42B53C70-E59B-4757-99CF-9D169C92385B}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="V36" sqref="V36"/>
+    <sheetView topLeftCell="P28" workbookViewId="0">
+      <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -20443,66 +20409,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -20510,67 +20466,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -22841,6 +22797,12 @@
       </c>
       <c r="W36" s="16">
         <v>4.55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37">
+        <f>SUM(E5:E35)/31</f>
+        <v>29.575806451612909</v>
       </c>
     </row>
   </sheetData>
@@ -22863,8 +22825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B5AAE48-C411-4E25-8B1D-2232EA02C65B}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="C32" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="L25" workbookViewId="0">
+      <selection activeCell="X37" sqref="X37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -22877,66 +22839,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -22944,67 +22896,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -25297,8 +25249,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E413A142-C323-471B-8DE8-71C83ABC936E}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="S25" workbookViewId="0">
+      <selection activeCell="Y35" sqref="Y35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -25311,66 +25263,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -25378,67 +25320,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -25959,7 +25901,7 @@
         <v>29</v>
       </c>
       <c r="F12" s="5">
-        <v>20.03</v>
+        <v>29.03</v>
       </c>
       <c r="G12" s="1">
         <v>35</v>
@@ -26882,7 +26824,7 @@
         <v>30.28</v>
       </c>
       <c r="F25" s="5">
-        <v>30.26</v>
+        <v>30.36</v>
       </c>
       <c r="G25" s="1">
         <v>37.200000000000003</v>
@@ -27729,9 +27671,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB82F61C-05AA-4FA3-BD74-74225C388CDC}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="B31" workbookViewId="0">
+    <sheetView topLeftCell="N25" workbookViewId="0">
       <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
@@ -27745,66 +27687,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -27812,67 +27744,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -29248,7 +29180,7 @@
         <v>30.5</v>
       </c>
       <c r="G24" s="1">
-        <v>38.799999999999997</v>
+        <v>30.8</v>
       </c>
       <c r="H24" s="1">
         <v>30</v>
@@ -30143,6 +30075,12 @@
       </c>
       <c r="W36" s="16">
         <v>2.78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37">
+        <f>SUM(E5:E35)/31</f>
+        <v>29.623548387096783</v>
       </c>
     </row>
   </sheetData>
@@ -30165,7 +30103,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FBA7423-C2C7-4634-AC7C-BDA41601DD7D}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
+    <sheetView topLeftCell="R25" workbookViewId="0">
       <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
@@ -30179,66 +30117,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -30246,67 +30174,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -30756,7 +30684,7 @@
         <v>29.51</v>
       </c>
       <c r="F11" s="5">
-        <v>20.11</v>
+        <v>29.11</v>
       </c>
       <c r="G11" s="1">
         <v>49.4</v>
@@ -32600,7 +32528,7 @@
   <dimension ref="A2:W36"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -32613,66 +32541,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -32680,67 +32598,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -35032,11 +34950,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CBB8FD-655A-4863-88F4-7CCF8E717079}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <pane ySplit="3" topLeftCell="M32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="W37" sqref="W37"/>
       <selection activeCell="O35" sqref="O35"/>
     </sheetView>
   </sheetViews>
@@ -35056,66 +34974,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -35123,67 +35031,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -37408,7 +37316,7 @@
         <v>34.6</v>
       </c>
       <c r="H36" s="14">
-        <v>24.6</v>
+        <v>34.6</v>
       </c>
       <c r="I36" s="14">
         <v>28.6</v>
@@ -37455,6 +37363,31 @@
       <c r="W36" s="16">
         <v>4.99</v>
       </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37"/>
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>28.471612903225804</v>
+      </c>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37">
+        <f>SUM(N5:N35)/31</f>
+        <v>0.17061290322580647</v>
+      </c>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="R37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -37475,9 +37408,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85204B69-BD73-463D-846C-48564885D419}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" workbookViewId="0">
+    <sheetView topLeftCell="N25" workbookViewId="0">
       <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
@@ -37491,66 +37424,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -37558,67 +37481,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -39889,6 +39812,12 @@
       </c>
       <c r="W36" s="16">
         <v>10.39</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.632903225806452</v>
       </c>
     </row>
   </sheetData>
@@ -39909,10 +39838,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8320C5D-44A6-4787-84A6-B2499FADF3C6}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="B33" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="B25" workbookViewId="0">
+      <selection activeCell="Y33" sqref="Y33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -39925,66 +39854,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -39992,67 +39911,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -41564,10 +41483,10 @@
         <v>22</v>
       </c>
       <c r="E26" s="4">
-        <v>29.44</v>
+        <v>30.44</v>
       </c>
       <c r="F26" s="5">
-        <v>29.38</v>
+        <v>30.38</v>
       </c>
       <c r="G26" s="1">
         <v>28.8</v>
@@ -41902,7 +41821,7 @@
         <v>10</v>
       </c>
       <c r="W30" s="11">
-        <v>0.03</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="31" spans="1:23" s="1" customFormat="1">
@@ -42044,7 +41963,7 @@
         <v>7</v>
       </c>
       <c r="W32" s="11">
-        <v>0.1</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="33" spans="1:23" s="1" customFormat="1">
@@ -42132,7 +42051,7 @@
         <v>30</v>
       </c>
       <c r="E34" s="4">
-        <v>29.54</v>
+        <v>28.54</v>
       </c>
       <c r="F34" s="5">
         <v>28.71</v>
@@ -42323,6 +42242,20 @@
       </c>
       <c r="W36" s="16">
         <v>3.35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37">
+        <f>SUM(E5:E35)/31</f>
+        <v>29.53</v>
+      </c>
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.534838709677423</v>
+      </c>
+      <c r="P37">
+        <f>SUM(P5:P35)/31</f>
+        <v>90.032258064516128</v>
       </c>
     </row>
   </sheetData>
@@ -42343,10 +42276,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2D07B89-795F-47D1-B9D9-3952301305F5}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="P25" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -42359,66 +42292,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -42426,67 +42349,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -44757,6 +44680,16 @@
       </c>
       <c r="W36" s="16">
         <v>5.84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37">
+        <f>SUM(E5:E35)/31</f>
+        <v>29.501612903225805</v>
+      </c>
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.51774193548388</v>
       </c>
     </row>
   </sheetData>
@@ -44777,10 +44710,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF3123BD-0C11-44C5-98B9-64CC39BFEE8C}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="B32" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -44793,66 +44726,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -44860,67 +44783,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -45095,7 +45018,7 @@
         <v>37</v>
       </c>
       <c r="I7" s="1">
-        <v>2</v>
+        <v>26</v>
       </c>
       <c r="J7" s="5">
         <v>38</v>
@@ -45722,7 +45645,7 @@
         <v>12</v>
       </c>
       <c r="E16" s="4">
-        <v>29.94</v>
+        <v>28.94</v>
       </c>
       <c r="F16" s="5">
         <v>28.94</v>
@@ -45793,10 +45716,10 @@
         <v>13</v>
       </c>
       <c r="E17" s="4">
-        <v>29.73</v>
+        <v>28.73</v>
       </c>
       <c r="F17" s="5">
-        <v>29.57</v>
+        <v>28.57</v>
       </c>
       <c r="G17" s="1">
         <v>36</v>
@@ -45864,7 +45787,7 @@
         <v>14</v>
       </c>
       <c r="E18" s="4">
-        <v>29.63</v>
+        <v>28.63</v>
       </c>
       <c r="F18" s="5">
         <v>28.67</v>
@@ -45935,7 +45858,7 @@
         <v>15</v>
       </c>
       <c r="E19" s="4">
-        <v>29.55</v>
+        <v>28.55</v>
       </c>
       <c r="F19" s="5">
         <v>29.05</v>
@@ -47191,6 +47114,16 @@
       </c>
       <c r="W36" s="16">
         <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.085161290322585</v>
+      </c>
+      <c r="P37">
+        <f>SUM(P5:P35)/31</f>
+        <v>88.225806451612897</v>
       </c>
     </row>
   </sheetData>
@@ -47213,8 +47146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C2E6BE9-1CB1-46BB-B103-F378C28219E9}">
   <dimension ref="A2:W36"/>
   <sheetViews>
-    <sheetView topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="E37" sqref="E37"/>
+    <sheetView topLeftCell="O25" workbookViewId="0">
+      <selection activeCell="W37" sqref="W37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -47227,66 +47160,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -47294,67 +47217,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -48798,7 +48721,7 @@
         <v>30.38</v>
       </c>
       <c r="F25" s="5">
-        <v>39.47</v>
+        <v>30.47</v>
       </c>
       <c r="G25" s="1">
         <v>41.1</v>
@@ -48890,7 +48813,7 @@
         <v>0.8</v>
       </c>
       <c r="M26" s="4">
-        <v>0.1787</v>
+        <v>0.17</v>
       </c>
       <c r="N26" s="5">
         <v>0.182</v>
@@ -49437,7 +49360,7 @@
         <v>28.8</v>
       </c>
       <c r="F34" s="5">
-        <v>29.94</v>
+        <v>28.94</v>
       </c>
       <c r="G34" s="1">
         <v>47.7</v>
@@ -49645,10 +49568,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E0FE9D5-A80F-41C9-AEC8-6E2C403BE377}">
-  <dimension ref="A2:W36"/>
+  <dimension ref="A2:W37"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="W37" sqref="W37"/>
+    <sheetView topLeftCell="B32" workbookViewId="0">
+      <selection activeCell="V37" sqref="V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -49661,66 +49584,56 @@
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="29"/>
-      <c r="G2" s="30" t="s">
+      <c r="F2" s="28"/>
+      <c r="G2" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="30"/>
-      <c r="I2" s="30"/>
-      <c r="J2" s="31"/>
-      <c r="K2" s="26" t="s">
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
+      <c r="K2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="L2" s="30"/>
-      <c r="M2" s="30"/>
-      <c r="N2" s="30"/>
-      <c r="O2" s="30"/>
-      <c r="P2" s="31"/>
-      <c r="Q2" s="30" t="s">
+      <c r="L2" s="29"/>
+      <c r="M2" s="29"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="30"/>
+      <c r="Q2" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="R2" s="30"/>
-      <c r="S2" s="30"/>
-      <c r="T2" s="31"/>
-      <c r="U2" s="26" t="s">
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="30"/>
+      <c r="U2" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="27"/>
+      <c r="V2" s="26"/>
       <c r="W2" s="9" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:23" s="2" customFormat="1">
       <c r="A3" s="3"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
       <c r="E3" s="17"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="24"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="24"/>
-      <c r="J3" s="25"/>
-      <c r="K3" s="32" t="s">
+      <c r="J3" s="24"/>
+      <c r="K3" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="L3" s="33"/>
-      <c r="M3" s="32" t="s">
+      <c r="L3" s="32"/>
+      <c r="M3" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="N3" s="33"/>
-      <c r="O3" s="34" t="s">
+      <c r="N3" s="32"/>
+      <c r="O3" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="35"/>
-      <c r="Q3" s="24"/>
-      <c r="R3" s="24"/>
-      <c r="S3" s="24"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="24"/>
+      <c r="P3" s="34"/>
+      <c r="T3" s="24"/>
       <c r="V3" s="1"/>
       <c r="W3" s="19"/>
     </row>
@@ -49728,67 +49641,67 @@
       <c r="A4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="24" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="24" t="s">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="24" t="s">
+      <c r="I4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="25" t="s">
+      <c r="J4" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="K4" s="24" t="s">
+      <c r="K4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="L4" s="25" t="s">
+      <c r="L4" s="24" t="s">
         <v>14</v>
       </c>
       <c r="M4" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="N4" s="25" t="s">
+      <c r="N4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P4" s="25" t="s">
+      <c r="P4" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="Q4" s="24" t="s">
+      <c r="Q4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R4" s="24" t="s">
+      <c r="R4" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S4" s="24" t="s">
+      <c r="S4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T4" s="25" t="s">
+      <c r="T4" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="U4" s="24" t="s">
+      <c r="U4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="V4" s="24" t="s">
+      <c r="V4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="W4" s="10" t="s">
@@ -50164,7 +50077,7 @@
         <v>6</v>
       </c>
       <c r="E10" s="4">
-        <v>29.82</v>
+        <v>29.62</v>
       </c>
       <c r="F10" s="5">
         <v>29.78</v>
@@ -50344,7 +50257,7 @@
       <c r="Q12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R12" s="20" t="s">
+      <c r="R12" s="35" t="s">
         <v>63</v>
       </c>
       <c r="S12" s="1" t="s">
@@ -50415,7 +50328,7 @@
       <c r="Q13" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="R13" s="20" t="s">
+      <c r="R13" s="35" t="s">
         <v>64</v>
       </c>
       <c r="S13" s="1" t="s">
@@ -51125,7 +51038,7 @@
       <c r="Q23" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="R23" s="20" t="s">
+      <c r="R23" s="35" t="s">
         <v>60</v>
       </c>
       <c r="S23" s="1" t="s">
@@ -51693,7 +51606,7 @@
       <c r="Q31" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R31" s="20" t="s">
+      <c r="R31" s="35" t="s">
         <v>63</v>
       </c>
       <c r="S31" s="1" t="s">
@@ -51764,7 +51677,7 @@
       <c r="Q32" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="R32" s="20" t="s">
+      <c r="R32" s="35" t="s">
         <v>60</v>
       </c>
       <c r="S32" s="1" t="s">
@@ -51835,7 +51748,7 @@
       <c r="Q33" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="R33" s="20" t="s">
+      <c r="R33" s="35" t="s">
         <v>66</v>
       </c>
       <c r="S33" s="1" t="s">
@@ -51906,7 +51819,7 @@
       <c r="Q34" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="R34" s="20" t="s">
+      <c r="R34" s="35" t="s">
         <v>63</v>
       </c>
       <c r="S34" s="1" t="s">
@@ -51977,7 +51890,7 @@
       <c r="Q35" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="R35" s="20" t="s">
+      <c r="R35" s="36" t="s">
         <v>61</v>
       </c>
       <c r="S35" s="7" t="s">
@@ -52042,7 +51955,7 @@
       <c r="Q36" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="R36" s="14">
+      <c r="R36" s="7">
         <v>3.7</v>
       </c>
       <c r="S36" s="14" t="s">
@@ -52059,6 +51972,16 @@
       </c>
       <c r="W36" s="16">
         <v>5.4009999999999998</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23">
+      <c r="E37">
+        <f>SUM(E5:E35)/31</f>
+        <v>29.610000000000003</v>
+      </c>
+      <c r="F37">
+        <f>SUM(F5:F35)/31</f>
+        <v>29.607741935483869</v>
       </c>
     </row>
   </sheetData>
@@ -52128,37 +52051,8 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Preview xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Preview>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_Flow_SignoffStatus xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xsi:nil="true"/>
-    <_dlc_DocId xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">H7Q62YT2XCZT-908671883-35274</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">
-      <Url>https://metoffice.sharepoint.com/sites/metofficelibraryarchiveteam/_layouts/15/DocIdRedir.aspx?ID=H7Q62YT2XCZT-908671883-35274</Url>
-      <Description>H7Q62YT2XCZT-908671883-35274</Description>
-    </_dlc_DocIdUrl>
-    <TaxCatchAll xmlns="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100005F0ACF65EC5C4F8622AE277C35A390" ma:contentTypeVersion="20" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="a11f18feb37c278a512788b2e5a06b2f">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xmlns:ns3="502a79df-4f52-4757-ac2f-753e065f4c93" xmlns:ns4="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d97308c79b2bb5835a55e257627f43a5" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100005F0ACF65EC5C4F8622AE277C35A390" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="7a4f56144ecba6ff6a413504c0ec2b8c">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xmlns:ns3="502a79df-4f52-4757-ac2f-753e065f4c93" xmlns:ns4="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7dcae21ac380e060fa17aa32c946feec" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="09baef80-0d7a-4cab-b988-bb3d9fc0663b"/>
     <xsd:import namespace="502a79df-4f52-4757-ac2f-753e065f4c93"/>
@@ -52190,6 +52084,8 @@
                 <xsd:element ref="ns2:MediaServiceLocation" minOccurs="0"/>
                 <xsd:element ref="ns4:TaxCatchAll" minOccurs="0"/>
                 <xsd:element ref="ns2:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceObjectDetectorVersions" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceSearchProperties" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -52288,6 +52184,16 @@
     <xsd:element name="MediaLengthInSeconds" ma:index="29" nillable="true" ma:displayName="MediaLengthInSeconds" ma:hidden="true" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceObjectDetectorVersions" ma:index="30" nillable="true" ma:displayName="MediaServiceObjectDetectorVersions" ma:hidden="true" ma:indexed="true" ma:internalName="MediaServiceObjectDetectorVersions" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceSearchProperties" ma:index="31" nillable="true" ma:displayName="MediaServiceSearchProperties" ma:hidden="true" ma:internalName="MediaServiceSearchProperties" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -52457,12 +52363,41 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Preview xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Preview>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_Flow_SignoffStatus xmlns="09baef80-0d7a-4cab-b988-bb3d9fc0663b" xsi:nil="true"/>
+    <_dlc_DocId xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">H7Q62YT2XCZT-908671883-35274</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="502a79df-4f52-4757-ac2f-753e065f4c93">
+      <Url>https://metoffice.sharepoint.com/sites/metofficelibraryarchiveteam/_layouts/15/DocIdRedir.aspx?ID=H7Q62YT2XCZT-908671883-35274</Url>
+      <Description>H7Q62YT2XCZT-908671883-35274</Description>
+    </_dlc_DocIdUrl>
+    <TaxCatchAll xmlns="95a6d21c-7db0-4b7e-981f-b4f22b02b9d8" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9C56BDC2-96B6-4F10-B70E-18812DB44A49}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37504570-BFED-402B-9995-BC94451CA335}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFD92123-871D-4582-BD87-22E616546C7A}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -52470,5 +52405,5 @@
 </file>
 
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B8560FE4-72CA-4675-82F8-49557EB78794}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{37504570-BFED-402B-9995-BC94451CA335}"/>
 </file>
</xml_diff>